<commit_message>
Version 2019.03.19 - Fixed bug when security name doesn't match between business units
</commit_message>
<xml_diff>
--- a/Actor-Security-Role-Reporter/Resources/ActorSecurityRoleReport.xlsx
+++ b/Actor-Security-Role-Reporter/Resources/ActorSecurityRoleReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -4165,7 +4165,69 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="D1:E3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
@@ -4226,8 +4288,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
   <location ref="J1:L3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -4286,8 +4348,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="F2:G4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -4358,70 +4420,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="D1:E3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="1">
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="1">
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="1">
-        <item x="0"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Name" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:A8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -4485,7 +4485,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E5:E8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -4545,7 +4545,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:A9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -4613,7 +4613,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
@@ -5004,7 +5004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -5242,7 +5242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>